<commit_message>
New pinouts for everything per the excel spreadsheet in the robockey folder. All the pins are set up but not necessarily used anywhere
</commit_message>
<xml_diff>
--- a/robockey/robockeyPins.xlsx
+++ b/robockey/robockeyPins.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="24480" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-140" windowWidth="10040" windowHeight="16220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pins Used" sheetId="2" r:id="rId1"/>
     <sheet name="MAEVARM Pins" sheetId="1" r:id="rId2"/>
+    <sheet name="Pins Used Old" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pins Used'!$A$1:$D$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pins Used Old'!$A$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="223">
   <si>
     <r>
       <t>GPIO port E, bit 6; pull-up optional; connected to </t>
@@ -155,19 +157,57 @@
     <t>TDO</t>
   </si>
   <si>
-    <t xml:space="preserve">PING Trigger </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PING Sense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaEvArM-pins</t>
-  </si>
-  <si>
-    <t>TO BE REPLACED WITH ADC 
-AFTER ADDING NOT GATE</t>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Motor 2 Direction</t>
+  </si>
+  <si>
+    <t>Motor 1 Direction</t>
+  </si>
+  <si>
+    <t>Motor 1 PWM</t>
+  </si>
+  <si>
+    <t>Motor 2 PWM</t>
+  </si>
+  <si>
+    <t>Would be ADC ref</t>
+  </si>
+  <si>
+    <t>PING trigger</t>
+  </si>
+  <si>
+    <t>PING sense</t>
+  </si>
+  <si>
+    <t>ptr</t>
+  </si>
+  <si>
+    <t>puck</t>
+  </si>
+  <si>
+    <t>LED 1</t>
+  </si>
+  <si>
+    <t>LED 2</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>ptr range</t>
+  </si>
+  <si>
+    <t>ptr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -600,7 +640,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Motor 2 Encoder B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Output</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEBUG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -722,12 +770,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -842,7 +884,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -880,7 +922,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -888,6 +929,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1211,40 +1257,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="7" customWidth="1"/>
     <col min="4" max="4" width="23" style="7" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1">
+    <row r="1" spans="1:6" ht="39" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E1" s="8"/>
-      <c r="H1" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="25" customHeight="1">
+      <c r="F1" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25" customHeight="1">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -1252,224 +1297,206 @@
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25" customHeight="1">
       <c r="A3" s="8">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="25" customHeight="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25" customHeight="1">
       <c r="A4" s="8">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="H4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="25" customHeight="1">
+        <v>163</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1">
       <c r="A5" s="8">
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="25" customHeight="1">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" customHeight="1">
       <c r="A6" s="8">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" customHeight="1">
       <c r="A7" s="8">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="36" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" customHeight="1">
       <c r="A8" s="8">
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="25" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" customHeight="1">
       <c r="A9" s="8">
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="25" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25" customHeight="1">
       <c r="A10" s="8">
         <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="25" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25" customHeight="1">
       <c r="A11" s="8">
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="25" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25" customHeight="1">
       <c r="A12" s="8">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="25" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25" customHeight="1">
       <c r="A13" s="8">
         <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="25" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25" customHeight="1">
       <c r="A14" s="8">
         <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="25" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25" customHeight="1">
       <c r="A15" s="8">
         <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="25" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" customHeight="1">
       <c r="A16" s="8">
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25" customHeight="1">
@@ -1477,10 +1504,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>128</v>
+        <v>47</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25" customHeight="1">
@@ -1488,13 +1518,13 @@
         <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25" customHeight="1">
@@ -1502,10 +1532,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>128</v>
+        <v>48</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25" customHeight="1">
@@ -1513,10 +1546,13 @@
         <v>26</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25" customHeight="1">
@@ -1524,13 +1560,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25" customHeight="1">
@@ -1541,7 +1577,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25" customHeight="1">
@@ -1552,7 +1591,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25" customHeight="1">
@@ -1563,7 +1605,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25" customHeight="1">
@@ -1574,7 +1619,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25" customHeight="1">
@@ -1585,7 +1633,10 @@
         <v>27</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="25" customHeight="1">
@@ -1593,10 +1644,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1606,7 +1660,6 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -1618,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1629,205 +1682,202 @@
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="10" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="11"/>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="10" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="10" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="11"/>
       <c r="B11" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="10" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30">
       <c r="A17" s="10" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15">
       <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" s="11"/>
       <c r="B19" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
       <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30">
       <c r="A21" s="10" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -1986,480 +2036,492 @@
         <v>31</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="10" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="11"/>
       <c r="B39" s="2" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26">
       <c r="A40" s="12"/>
       <c r="B40" s="2" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="10" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" s="11"/>
       <c r="B42" s="2" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15">
       <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15">
       <c r="A44" s="10" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15">
       <c r="A45" s="11"/>
       <c r="B45" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15">
       <c r="A46" s="12"/>
       <c r="B46" s="2" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15">
       <c r="A47" s="10" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15">
       <c r="A48" s="11"/>
       <c r="B48" s="2" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15">
       <c r="A49" s="11"/>
       <c r="B49" s="2" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15">
       <c r="A50" s="12"/>
       <c r="B50" s="2" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15">
       <c r="A51" s="10" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15">
       <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15">
       <c r="A53" s="11"/>
       <c r="B53" s="2" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15">
       <c r="A54" s="12"/>
       <c r="B54" s="2" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15">
       <c r="A55" s="10" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15">
       <c r="A56" s="11"/>
       <c r="B56" s="2" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15">
       <c r="A57" s="11"/>
       <c r="B57" s="2" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15">
       <c r="A58" s="11"/>
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15">
       <c r="A59" s="12"/>
       <c r="B59" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="30">
       <c r="A60" s="10" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15">
       <c r="A61" s="11"/>
       <c r="B61" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15">
       <c r="A62" s="11"/>
       <c r="B62" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15">
       <c r="A63" s="12"/>
       <c r="B63" s="2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30">
       <c r="A64" s="10" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15">
       <c r="A65" s="11"/>
       <c r="B65" s="2" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15">
       <c r="A66" s="12"/>
       <c r="B66" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15">
       <c r="A67" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15">
       <c r="A68" s="11"/>
       <c r="B68" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15">
       <c r="A69" s="12"/>
       <c r="B69" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15">
       <c r="A70" s="10" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15">
       <c r="A71" s="11"/>
       <c r="B71" s="2" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15">
       <c r="A72" s="12"/>
       <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15">
       <c r="A73" s="10" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15">
       <c r="A74" s="11"/>
       <c r="B74" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15">
       <c r="A75" s="12"/>
       <c r="B75" s="2" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15">
       <c r="A76" s="10" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15">
       <c r="A77" s="11"/>
       <c r="B77" s="2" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15">
       <c r="A78" s="12"/>
       <c r="B78" s="2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15">
       <c r="A79" s="10" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15">
       <c r="A80" s="11"/>
       <c r="B80" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15">
       <c r="A81" s="11"/>
       <c r="B81" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15">
       <c r="A82" s="12"/>
       <c r="B82" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15">
       <c r="A83" s="10" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15">
       <c r="A84" s="11"/>
       <c r="B84" s="2" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15">
       <c r="A85" s="11"/>
       <c r="B85" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15">
       <c r="A86" s="12"/>
       <c r="B86" s="2" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A79:A82"/>
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A4:A8"/>
@@ -2473,18 +2535,6 @@
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A79:A82"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2492,7 +2542,6 @@
     <hyperlink ref="C34" r:id="rId2"/>
     <hyperlink ref="C37" r:id="rId3"/>
     <hyperlink ref="C40" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2501,4 +2550,403 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="39" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25" customHeight="1">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25" customHeight="1">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25" customHeight="1">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25" customHeight="1">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" customHeight="1">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" customHeight="1">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" customHeight="1">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25" customHeight="1">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25" customHeight="1">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25" customHeight="1">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25" customHeight="1">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25" customHeight="1">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25" customHeight="1">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25" customHeight="1">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25" customHeight="1">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="25" customHeight="1">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25" customHeight="1">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="25" customHeight="1">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25" customHeight="1">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="25" customHeight="1">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25" customHeight="1">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25" customHeight="1">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25" customHeight="1">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25" customHeight="1">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25" customHeight="1">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D27"/>
+  <sortState ref="A2:D27">
+    <sortCondition ref="A2:A27"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>